<commit_message>
Added more methods for clustering.
</commit_message>
<xml_diff>
--- a/data/output/cluster_metrics_kmeans.xlsx
+++ b/data/output/cluster_metrics_kmeans.xlsx
@@ -485,8 +485,10 @@
           <t>qa_coverage_line_%</t>
         </is>
       </c>
-      <c r="F2" t="n">
-        <v>1.180130815367262e-14</v>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>1.18e-14</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -509,8 +511,10 @@
           <t>qa_coverage_line_%</t>
         </is>
       </c>
-      <c r="F3" t="n">
-        <v>1.634871885687534e-13</v>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>1.63e-13</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -533,8 +537,10 @@
           <t>qa_coverage_line_%</t>
         </is>
       </c>
-      <c r="F4" t="n">
-        <v>3.811713889470054e-16</v>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>3.81e-16</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -557,8 +563,10 @@
           <t>qa_fix_dispersion_mean</t>
         </is>
       </c>
-      <c r="F5" t="n">
-        <v>3.611879109083059e-14</v>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>3.61e-14</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -581,8 +589,10 @@
           <t>qa_dwell_time_pdf</t>
         </is>
       </c>
-      <c r="F6" t="n">
-        <v>2.16972029118715e-21</v>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2.17e-21</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -605,8 +615,10 @@
           <t>qa_coverage_line_%</t>
         </is>
       </c>
-      <c r="F7" t="n">
-        <v>1.443183436653568e-10</v>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>1.44e-10</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -629,8 +641,10 @@
           <t>qa_coverage_line_%</t>
         </is>
       </c>
-      <c r="F8" t="n">
-        <v>8.745205101910946e-17</v>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>8.75e-17</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>